<commit_message>
Getting Somewhere, Doing Updated Algorithm TOMORROW, TOMORROW, TOMORROW
</commit_message>
<xml_diff>
--- a/Week 18/ScoredBaseline-3-9.xlsx
+++ b/Week 18/ScoredBaseline-3-9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbeln\OneDrive\Documents\UF\Research\Week 18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263DCB50-3D38-4C93-9809-766253462FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990F1FD4-EF6D-41A8-BC5E-9B2F7F9CB907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="11512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,16 +293,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -315,6 +307,26 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Atlas Grotesk Regular"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Atlas Grotesk Regular"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Atlas Grotesk Regular"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -351,18 +363,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -670,23 +683,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="29" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="48.3984375" customWidth="1"/>
-    <col min="5" max="5" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.3984375" style="3" customWidth="1"/>
+    <col min="2" max="4" width="9.06640625" style="3"/>
+    <col min="5" max="6" width="15.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,943 +731,943 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>0.52065972222222223</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>0.22222222222222221</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>0.55555555555555547</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
         <v>0.703125</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.51250000000000007</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>0.4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>0.42499999999999999</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>0.7</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
         <v>0.56666666666666676</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.50960648148148147</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.22222222222222221</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.48148148148148151</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
         <v>0.46875</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.47083333333333333</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.2857142857142857</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>0.2857142857142857</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>0.6607142857142857</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>0.5714285714285714</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
         <v>0.44444444444444448</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>0.4634166666666667</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0.16666666666666671</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>0.5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>0.4375</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
         <v>0.51</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.43598484848484848</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.1818181818181818</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.2121212121212121</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>0.375</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>0.72727272727272718</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
         <v>0.5</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>0.37611111111111112</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>0.2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>0.3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>0.35</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>0.53333333333333333</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
         <v>0.32592592592592601</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>0.37013888888888891</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>0.27777777777777768</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>0.47916666666666669</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>0.94444444444444431</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>0.35045454545454552</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
         <v>0.2121212121212121</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>0.26136363636363641</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>0.60606060606060597</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
         <v>0.47499999999999998</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>0.3363888888888889</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>0.16666666666666671</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>0.38888888888888878</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>0.66666666666666674</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>0.2</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>0.32275757575757569</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>0.38636363636363641</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>0.51515151515151514</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
         <v>0.24</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>0.31013818027210888</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
         <v>0.125</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>0.484375</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>0.70833333333333326</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
         <v>0.26122448979591839</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>0.30833333333333329</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
         <v>0.80952380952380942</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>0.32142857142857151</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>0.95238095238095244</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>0.28958333333333341</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
         <v>0.6333333333333333</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>0.46250000000000002</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>0.8</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>0.28583333333333327</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>0.2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0.42499999999999999</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>0.3</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
         <v>0.16666666666666671</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>0.28379629629629632</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>0.1111111111111111</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>0.37037037037037029</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0.43055555555555558</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>0.70370370370370372</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>0.23154761904761911</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
         <v>0.33333333333333343</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>0.4107142857142857</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>0.5714285714285714</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>0.18583333333333341</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
         <v>0.1333333333333333</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>0.32500000000000001</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>0.4</v>
       </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>0.17805555555555561</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
         <v>0.17777777777777781</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>0.22500000000000001</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>0.37777777777777771</v>
       </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>0.17326388888888891</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
         <v>0.59375</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>0.1388888888888889</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
         <v>0.375</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>0.484375</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>0.125</v>
       </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
         <v>0.14814814814814811</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>0.18055555555555561</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>0.37037037037037041</v>
       </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="I23" s="3">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
         <v>0.26785714285714279</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>4.7619047619047623E-2</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
         <v>9.5238095238095233E-2</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>0.5178571428571429</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>0.15384615384615391</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>0.42307692307692307</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
         <v>0.1</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>0.4</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>0.28749999999999998</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>0.6</v>
       </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.65">
+      <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
         <v>0.40740740740740738</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>0.5</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>0.14814814814814811</v>
       </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>